<commit_message>
update from svn 12-07-2013
</commit_message>
<xml_diff>
--- a/documents/Agendas/201401 WGM FHIR Agenda.xlsx
+++ b/documents/Agendas/201401 WGM FHIR Agenda.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="62">
   <si>
     <t>Sat</t>
   </si>
@@ -96,9 +96,6 @@
     <t>PC</t>
   </si>
   <si>
-    <t>PA?</t>
-  </si>
-  <si>
     <t>PHER</t>
   </si>
   <si>
@@ -108,127 +105,110 @@
     <t>SD</t>
   </si>
   <si>
+    <t>Vocab/MnM</t>
+  </si>
+  <si>
+    <t>OO</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>Devices</t>
+  </si>
+  <si>
+    <t>Mobile Health</t>
+  </si>
+  <si>
+    <t>Clinical Genomics</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Tutorial or ARB</t>
+  </si>
+  <si>
+    <t>II/DICOM</t>
+  </si>
+  <si>
+    <t>CDS</t>
+  </si>
+  <si>
+    <t>Electronic Services</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>MnM + ITS</t>
+  </si>
+  <si>
+    <t>EHR</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>Tooling/RIMBAA</t>
+  </si>
+  <si>
+    <t>Q5/Q6</t>
+  </si>
+  <si>
+    <t>Facilitator's roundtable</t>
+  </si>
+  <si>
+    <t>Q0</t>
+  </si>
+  <si>
+    <t>Tool Planning</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>TSC Report</t>
+  </si>
+  <si>
+    <t>InM</t>
+  </si>
+  <si>
+    <t>FMG</t>
+  </si>
+  <si>
+    <t>4-5</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>Tooling</t>
+  </si>
+  <si>
+    <t>free time  or FMG</t>
+  </si>
+  <si>
+    <t>free time or join roundtable</t>
+  </si>
+  <si>
+    <t>SOA, ITS</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>MnM?</t>
+  </si>
+  <si>
     <t>InM + ITS</t>
-  </si>
-  <si>
-    <t>Vocab/MnM</t>
-  </si>
-  <si>
-    <t>OO</t>
-  </si>
-  <si>
-    <t>FM</t>
-  </si>
-  <si>
-    <t>Devices</t>
-  </si>
-  <si>
-    <t>Mobile Health</t>
-  </si>
-  <si>
-    <t>Clinical Genomics</t>
-  </si>
-  <si>
-    <t>Security</t>
-  </si>
-  <si>
-    <t>Tutorial or ARB</t>
-  </si>
-  <si>
-    <t>II/DICOM</t>
-  </si>
-  <si>
-    <t>CDS</t>
-  </si>
-  <si>
-    <t>Electronic Services</t>
-  </si>
-  <si>
-    <t>Education</t>
-  </si>
-  <si>
-    <t>MnM + ITS</t>
-  </si>
-  <si>
-    <t>Devices??</t>
-  </si>
-  <si>
-    <t>EHR</t>
-  </si>
-  <si>
-    <t>CDS?</t>
-  </si>
-  <si>
-    <t>Q6</t>
-  </si>
-  <si>
-    <t>Tooling/RIMBAA</t>
-  </si>
-  <si>
-    <t>Q5/Q6</t>
-  </si>
-  <si>
-    <t>Facilitator's roundtable</t>
-  </si>
-  <si>
-    <t>Q0</t>
-  </si>
-  <si>
-    <t>Tool Planning</t>
-  </si>
-  <si>
-    <t>Lunch</t>
-  </si>
-  <si>
-    <t>TSC Report</t>
-  </si>
-  <si>
-    <t>InM</t>
-  </si>
-  <si>
-    <t>FMG</t>
-  </si>
-  <si>
-    <t>4-5</t>
-  </si>
-  <si>
-    <t>1-2</t>
-  </si>
-  <si>
-    <t>Tooling</t>
-  </si>
-  <si>
-    <t>free time ;&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">MnM or </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SD?</t>
-    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,19 +224,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -271,13 +251,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,10 +564,10 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26:XFD26"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,7 +599,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -630,14 +612,14 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -650,14 +632,14 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -670,14 +652,14 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -690,14 +672,14 @@
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -710,14 +692,14 @@
       <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -728,12 +710,12 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G8" t="s">
@@ -750,14 +732,14 @@
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H9">
         <v>3</v>
@@ -770,14 +752,14 @@
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -790,14 +772,14 @@
       <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" t="s">
-        <v>54</v>
+      <c r="C11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -810,10 +792,10 @@
       <c r="B12" t="s">
         <v>1</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G12" t="s">
@@ -830,17 +812,17 @@
       <c r="B13" t="s">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D13" t="s">
-        <v>43</v>
+      <c r="D13" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="G13" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>57</v>
+      <c r="H13" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -848,15 +830,15 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D14" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="3"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -865,10 +847,10 @@
       <c r="B15" t="s">
         <v>3</v>
       </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>17</v>
       </c>
       <c r="G15" t="s">
@@ -885,17 +867,17 @@
       <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>17</v>
       </c>
       <c r="G16" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>58</v>
+      <c r="H16" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -905,11 +887,11 @@
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D17" t="s">
-        <v>21</v>
+      <c r="D17" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="G17" t="s">
         <v>23</v>
@@ -925,14 +907,14 @@
       <c r="B18" t="s">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>24</v>
       </c>
       <c r="G18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -945,14 +927,14 @@
       <c r="B19" t="s">
         <v>3</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D19" t="s">
-        <v>26</v>
+      <c r="D19" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="G19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -965,14 +947,14 @@
       <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D20" t="s">
-        <v>30</v>
+      <c r="D20" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="G20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -983,13 +965,13 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="G21" t="s">
         <v>21</v>
@@ -1005,14 +987,14 @@
       <c r="B22" t="s">
         <v>1</v>
       </c>
-      <c r="C22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" t="s">
-        <v>32</v>
+      <c r="C22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="G22" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1025,11 +1007,11 @@
       <c r="B23" t="s">
         <v>2</v>
       </c>
-      <c r="C23" t="s">
-        <v>31</v>
+      <c r="C23" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1039,11 +1021,11 @@
       <c r="B24" t="s">
         <v>3</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D24" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1053,11 +1035,11 @@
       <c r="B25" t="s">
         <v>4</v>
       </c>
-      <c r="C25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" t="s">
-        <v>28</v>
+      <c r="C25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1067,11 +1049,11 @@
       <c r="B26" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>37</v>
+      <c r="D26" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1081,11 +1063,11 @@
       <c r="B27" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" t="s">
-        <v>32</v>
+      <c r="C27" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1095,10 +1077,10 @@
       <c r="B28" t="s">
         <v>3</v>
       </c>
-      <c r="C28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1109,11 +1091,11 @@
       <c r="B29" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" t="s">
-        <v>39</v>
+      <c r="C29" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1121,13 +1103,13 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" t="s">
-        <v>60</v>
+        <v>45</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1135,13 +1117,13 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1151,25 +1133,28 @@
       <c r="B32" t="s">
         <v>1</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
       <c r="B33" t="s">
         <v>2</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>61</v>
+      <c r="D33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>